<commit_message>
Add LRU to presentation.
</commit_message>
<xml_diff>
--- a/Project2/figure/log.xlsx
+++ b/Project2/figure/log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8C0CD4-9334-4DA4-BBDA-CBB40DE8F123}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5639BAE4-C2A8-41DD-8256-37BE06C1B889}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>Active</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,6 +47,78 @@
   </si>
   <si>
     <t>MAX 0x80 THRESH 0x8</t>
+  </si>
+  <si>
+    <t>LRU offset 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Active</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inactive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x9</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x10</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x11</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x12</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x13</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x14</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x15</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x16</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x17</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x18</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x19</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x20</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x21</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x22</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x23</t>
+  </si>
+  <si>
+    <t>MAX 0x80 THRESH 0x24</t>
+  </si>
+  <si>
+    <t>LRU offset 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LRU offset 16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LRU offset 256</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1667,49 +1739,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>136</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>138</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>137</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>137</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>137</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>137</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>137</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>175</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>189</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>160</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>122</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>108</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>108</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>111</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>111</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2970,6 +3042,1610 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Variation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t> trend</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Active</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$39:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>617</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>914</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>932</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>136</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B72C-4DF2-B8E7-78BA4B45D5F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inactive</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$39:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B72C-4DF2-B8E7-78BA4B45D5F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="483361840"/>
+        <c:axId val="372600048"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="483361840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="372600048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="372600048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="483361840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Active list size with</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t> different O-T</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="58000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$39:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>587</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>833</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>898</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>926</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>943</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>138</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4CF0-454A-9681-0B7A85F0FEA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="86000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$39:$D$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>495</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>617</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>723</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>914</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>932</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>136</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4CF0-454A-9681-0B7A85F0FEA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="86000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$39:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>241</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>547</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>638</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>844</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>924</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>766</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>138</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-4CF0-454A-9681-0B7A85F0FEA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="58000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$39:$J$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>483</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>602</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>703</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>915</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>939</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>135</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4CF0-454A-9681-0B7A85F0FEA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="483361840"/>
+        <c:axId val="372600048"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="483361840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="372600048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="372600048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="483361840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Inactive list size with</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+              <a:t> different O-T</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="58000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$39:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6FC8-46CE-968A-F46D9E42DA0B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="86000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$39:$E$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-6FC8-46CE-968A-F46D9E42DA0B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="86000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$39:$H$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-6FC8-46CE-968A-F46D9E42DA0B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>8</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="58000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$39:$K$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-6FC8-46CE-968A-F46D9E42DA0B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="483361840"/>
+        <c:axId val="372600048"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="483361840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="372600048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="372600048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="483361840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
   <a:schemeClr val="accent1"/>
@@ -3000,6 +4676,24 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -5065,6 +6759,1554 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5734,16 +8976,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>8466</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>42334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>67733</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>118534</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5765,6 +9007,120 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>452967</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>29633</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="图表 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F03B7A6-B9C3-4F84-AB10-0E59CDD819CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>423334</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>143934</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>491067</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>42334</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="图表 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{795231C0-5A17-47B0-B483-0F705247B3C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>160866</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>486833</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>59266</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="图表 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C7C04E2-3B80-4714-906A-077D8AEA635D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6036,10 +9392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="S43" sqref="S43"/>
+    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
@@ -6400,7 +9756,7 @@
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H20" t="s">
         <v>1</v>
@@ -6419,8 +9775,8 @@
       <c r="E21">
         <v>250</v>
       </c>
-      <c r="G21">
-        <v>136</v>
+      <c r="G21" t="s">
+        <v>12</v>
       </c>
       <c r="H21">
         <v>255</v>
@@ -6439,8 +9795,8 @@
       <c r="E22">
         <v>358</v>
       </c>
-      <c r="G22">
-        <v>138</v>
+      <c r="G22" t="s">
+        <v>13</v>
       </c>
       <c r="H22">
         <v>276</v>
@@ -6459,8 +9815,8 @@
       <c r="E23">
         <v>442</v>
       </c>
-      <c r="G23">
-        <v>137</v>
+      <c r="G23" t="s">
+        <v>14</v>
       </c>
       <c r="H23">
         <v>357</v>
@@ -6479,8 +9835,8 @@
       <c r="E24">
         <v>497</v>
       </c>
-      <c r="G24">
-        <v>137</v>
+      <c r="G24" t="s">
+        <v>15</v>
       </c>
       <c r="H24">
         <v>449</v>
@@ -6499,8 +9855,8 @@
       <c r="E25">
         <v>604</v>
       </c>
-      <c r="G25">
-        <v>137</v>
+      <c r="G25" t="s">
+        <v>16</v>
       </c>
       <c r="H25">
         <v>562</v>
@@ -6519,8 +9875,8 @@
       <c r="E26">
         <v>694</v>
       </c>
-      <c r="G26">
-        <v>137</v>
+      <c r="G26" t="s">
+        <v>17</v>
       </c>
       <c r="H26">
         <v>677</v>
@@ -6539,8 +9895,8 @@
       <c r="E27">
         <v>794</v>
       </c>
-      <c r="G27">
-        <v>137</v>
+      <c r="G27" t="s">
+        <v>18</v>
       </c>
       <c r="H27">
         <v>788</v>
@@ -6559,8 +9915,8 @@
       <c r="E28">
         <v>843</v>
       </c>
-      <c r="G28">
-        <v>175</v>
+      <c r="G28" t="s">
+        <v>19</v>
       </c>
       <c r="H28">
         <v>798</v>
@@ -6579,8 +9935,8 @@
       <c r="E29">
         <v>805</v>
       </c>
-      <c r="G29">
-        <v>189</v>
+      <c r="G29" t="s">
+        <v>20</v>
       </c>
       <c r="H29">
         <v>784</v>
@@ -6599,8 +9955,8 @@
       <c r="E30">
         <v>832</v>
       </c>
-      <c r="G30">
-        <v>160</v>
+      <c r="G30" t="s">
+        <v>21</v>
       </c>
       <c r="H30">
         <v>816</v>
@@ -6619,8 +9975,8 @@
       <c r="E31">
         <v>854</v>
       </c>
-      <c r="G31">
-        <v>122</v>
+      <c r="G31" t="s">
+        <v>22</v>
       </c>
       <c r="H31">
         <v>848</v>
@@ -6639,14 +9995,14 @@
       <c r="E32">
         <v>155</v>
       </c>
-      <c r="G32">
-        <v>108</v>
+      <c r="G32" t="s">
+        <v>23</v>
       </c>
       <c r="H32">
         <v>617</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>98</v>
       </c>
@@ -6659,14 +10015,14 @@
       <c r="E33">
         <v>67</v>
       </c>
-      <c r="G33">
-        <v>108</v>
+      <c r="G33" t="s">
+        <v>24</v>
       </c>
       <c r="H33">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>101</v>
       </c>
@@ -6679,14 +10035,14 @@
       <c r="E34">
         <v>79</v>
       </c>
-      <c r="G34">
-        <v>111</v>
+      <c r="G34" t="s">
+        <v>25</v>
       </c>
       <c r="H34">
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>102</v>
       </c>
@@ -6699,11 +10055,389 @@
       <c r="E35">
         <v>82</v>
       </c>
-      <c r="G35">
-        <v>111</v>
+      <c r="G35" t="s">
+        <v>26</v>
       </c>
       <c r="H35">
         <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" t="s">
+        <v>28</v>
+      </c>
+      <c r="J37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J38" t="s">
+        <v>9</v>
+      </c>
+      <c r="K38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>161</v>
+      </c>
+      <c r="B39">
+        <v>193</v>
+      </c>
+      <c r="D39">
+        <v>159</v>
+      </c>
+      <c r="E39">
+        <v>200</v>
+      </c>
+      <c r="G39">
+        <v>161</v>
+      </c>
+      <c r="H39">
+        <v>191</v>
+      </c>
+      <c r="J39">
+        <v>160</v>
+      </c>
+      <c r="K39">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>228</v>
+      </c>
+      <c r="B40">
+        <v>193</v>
+      </c>
+      <c r="D40">
+        <v>245</v>
+      </c>
+      <c r="E40">
+        <v>200</v>
+      </c>
+      <c r="G40">
+        <v>241</v>
+      </c>
+      <c r="H40">
+        <v>191</v>
+      </c>
+      <c r="J40">
+        <v>247</v>
+      </c>
+      <c r="K40">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>334</v>
+      </c>
+      <c r="B41">
+        <v>193</v>
+      </c>
+      <c r="D41">
+        <v>376</v>
+      </c>
+      <c r="E41">
+        <v>200</v>
+      </c>
+      <c r="G41">
+        <v>361</v>
+      </c>
+      <c r="H41">
+        <v>191</v>
+      </c>
+      <c r="J41">
+        <v>374</v>
+      </c>
+      <c r="K41">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>460</v>
+      </c>
+      <c r="B42">
+        <v>193</v>
+      </c>
+      <c r="D42">
+        <v>495</v>
+      </c>
+      <c r="E42">
+        <v>200</v>
+      </c>
+      <c r="G42">
+        <v>480</v>
+      </c>
+      <c r="H42">
+        <v>191</v>
+      </c>
+      <c r="J42">
+        <v>483</v>
+      </c>
+      <c r="K42">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>587</v>
+      </c>
+      <c r="B43">
+        <v>193</v>
+      </c>
+      <c r="D43">
+        <v>617</v>
+      </c>
+      <c r="E43">
+        <v>200</v>
+      </c>
+      <c r="G43">
+        <v>547</v>
+      </c>
+      <c r="H43">
+        <v>191</v>
+      </c>
+      <c r="J43">
+        <v>602</v>
+      </c>
+      <c r="K43">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>715</v>
+      </c>
+      <c r="B44">
+        <v>193</v>
+      </c>
+      <c r="D44">
+        <v>723</v>
+      </c>
+      <c r="E44">
+        <v>200</v>
+      </c>
+      <c r="G44">
+        <v>638</v>
+      </c>
+      <c r="H44">
+        <v>191</v>
+      </c>
+      <c r="J44">
+        <v>703</v>
+      </c>
+      <c r="K44">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>833</v>
+      </c>
+      <c r="B45">
+        <v>144</v>
+      </c>
+      <c r="D45">
+        <v>810</v>
+      </c>
+      <c r="E45">
+        <v>165</v>
+      </c>
+      <c r="G45">
+        <v>756</v>
+      </c>
+      <c r="H45">
+        <v>191</v>
+      </c>
+      <c r="J45">
+        <v>785</v>
+      </c>
+      <c r="K45">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>898</v>
+      </c>
+      <c r="B46">
+        <v>78</v>
+      </c>
+      <c r="D46">
+        <v>889</v>
+      </c>
+      <c r="E46">
+        <v>86</v>
+      </c>
+      <c r="G46">
+        <v>844</v>
+      </c>
+      <c r="H46">
+        <v>130</v>
+      </c>
+      <c r="J46">
+        <v>880</v>
+      </c>
+      <c r="K46">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>926</v>
+      </c>
+      <c r="B47">
+        <v>51</v>
+      </c>
+      <c r="D47">
+        <v>914</v>
+      </c>
+      <c r="E47">
+        <v>64</v>
+      </c>
+      <c r="G47">
+        <v>896</v>
+      </c>
+      <c r="H47">
+        <v>76</v>
+      </c>
+      <c r="J47">
+        <v>915</v>
+      </c>
+      <c r="K47">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>943</v>
+      </c>
+      <c r="B48">
+        <v>34</v>
+      </c>
+      <c r="D48">
+        <v>932</v>
+      </c>
+      <c r="E48">
+        <v>48</v>
+      </c>
+      <c r="G48">
+        <v>924</v>
+      </c>
+      <c r="H48">
+        <v>54</v>
+      </c>
+      <c r="J48">
+        <v>939</v>
+      </c>
+      <c r="K48">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>135</v>
+      </c>
+      <c r="B49">
+        <v>39</v>
+      </c>
+      <c r="D49">
+        <v>133</v>
+      </c>
+      <c r="E49">
+        <v>54</v>
+      </c>
+      <c r="G49">
+        <v>766</v>
+      </c>
+      <c r="H49">
+        <v>39</v>
+      </c>
+      <c r="J49">
+        <v>950</v>
+      </c>
+      <c r="K49">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>136</v>
+      </c>
+      <c r="B50">
+        <v>41</v>
+      </c>
+      <c r="D50">
+        <v>136</v>
+      </c>
+      <c r="E50">
+        <v>63</v>
+      </c>
+      <c r="G50">
+        <v>136</v>
+      </c>
+      <c r="H50">
+        <v>44</v>
+      </c>
+      <c r="J50">
+        <v>134</v>
+      </c>
+      <c r="K50">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>138</v>
+      </c>
+      <c r="B51">
+        <v>52</v>
+      </c>
+      <c r="D51">
+        <v>136</v>
+      </c>
+      <c r="E51">
+        <v>68</v>
+      </c>
+      <c r="G51">
+        <v>138</v>
+      </c>
+      <c r="H51">
+        <v>52</v>
+      </c>
+      <c r="J51">
+        <v>135</v>
+      </c>
+      <c r="K51">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>